<commit_message>
Added Two new Features (i.e., No:2,10 from Clustering paper) And then moved all the code from test to scripts folder.
</commit_message>
<xml_diff>
--- a/results/Assignment_1_Results.xlsx
+++ b/results/Assignment_1_Results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,45 +446,50 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>FLC</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
           <t>NP</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>NC</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>NR</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>NFRec</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>NCRec</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>NIFPar</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>NRRec</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>NRNRec</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>Final_Score</t>
         </is>
@@ -500,17 +505,17 @@
         <v>3</v>
       </c>
       <c r="C2" t="n">
-        <v>3</v>
+        <v>15.75</v>
       </c>
       <c r="D2" t="n">
+        <v>3</v>
+      </c>
+      <c r="E2" t="n">
         <v>4</v>
       </c>
-      <c r="E2" t="n">
+      <c r="F2" t="n">
         <v>6</v>
       </c>
-      <c r="F2" t="n">
-        <v>1</v>
-      </c>
       <c r="G2" t="n">
         <v>1</v>
       </c>
@@ -523,7 +528,10 @@
       <c r="J2" t="n">
         <v>1</v>
       </c>
-      <c r="K2" t="inlineStr">
+      <c r="K2" t="n">
+        <v>1</v>
+      </c>
+      <c r="L2" t="inlineStr">
         <is>
           <t>100%</t>
         </is>
@@ -539,16 +547,16 @@
         <v>3</v>
       </c>
       <c r="C3" t="n">
-        <v>3</v>
+        <v>18.25</v>
       </c>
       <c r="D3" t="n">
         <v>3</v>
       </c>
       <c r="E3" t="n">
+        <v>3</v>
+      </c>
+      <c r="F3" t="n">
         <v>6</v>
-      </c>
-      <c r="F3" t="n">
-        <v>0</v>
       </c>
       <c r="G3" t="n">
         <v>0</v>
@@ -562,9 +570,12 @@
       <c r="J3" t="n">
         <v>0</v>
       </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>41.67%</t>
+      <c r="K3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>45.49%</t>
         </is>
       </c>
     </row>
@@ -578,32 +589,35 @@
         <v>3</v>
       </c>
       <c r="C4" t="n">
-        <v>3</v>
+        <v>18.25</v>
       </c>
       <c r="D4" t="n">
+        <v>3</v>
+      </c>
+      <c r="E4" t="n">
         <v>4</v>
       </c>
-      <c r="E4" t="n">
+      <c r="F4" t="n">
         <v>7</v>
       </c>
-      <c r="F4" t="n">
-        <v>1</v>
-      </c>
       <c r="G4" t="n">
         <v>1</v>
       </c>
       <c r="H4" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I4" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J4" t="n">
+        <v>1</v>
+      </c>
+      <c r="K4" t="n">
         <v>2</v>
       </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>75.46%</t>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>75.91%</t>
         </is>
       </c>
     </row>

</xml_diff>